<commit_message>
Change -999 to 0 in ratings
</commit_message>
<xml_diff>
--- a/PlayerRating.xlsx
+++ b/PlayerRating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Folder\Training\github\Python\Soccer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC313DE8-5591-48FA-B382-E0F8040E8739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FD00FF-2928-4404-BC1F-81F068BA5946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -449,7 +449,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,10 +476,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <v>5</v>
@@ -496,7 +496,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,7 +560,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -574,7 +574,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -588,7 +588,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -608,7 +608,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,7 +658,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
         <v>4</v>
@@ -672,7 +672,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -686,7 +686,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>-999</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>

</xml_diff>